<commit_message>
check export: PhieuPhanCa + BangCongNV
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/CaLamViec_ChamCong/Teamplate_DanhSachPhieuPhanCa.xlsx
+++ b/banhang24/Template/ExportExcel/CaLamViec_ChamCong/Teamplate_DanhSachPhieuPhanCa.xlsx
@@ -139,7 +139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -156,6 +156,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -165,11 +171,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -476,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,48 +499,48 @@
     <col min="1" max="1" width="14.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="17.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="16" style="10" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="7" customWidth="1"/>
     <col min="7" max="7" width="27.85546875" style="5" customWidth="1"/>
     <col min="8" max="8" width="30.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -540,13 +552,13 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -555,6 +567,46 @@
       <c r="H4" s="3" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>